<commit_message>
Updated page layout and added gantt.pdf
</commit_message>
<xml_diff>
--- a/documentation/gantt.xlsx
+++ b/documentation/gantt.xlsx
@@ -2959,7 +2959,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:S60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -4189,7 +4189,10 @@
     <mergeCell ref="P39:R39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="64" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="8" max="1048575" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>